<commit_message>
Fixed Database & Get Query
</commit_message>
<xml_diff>
--- a/public/DataMahasiswa/DatabaseMahasiswa.xlsx
+++ b/public/DataMahasiswa/DatabaseMahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F9417-B629-4A46-A430-21C343933A35}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD32F5A-798D-4ABD-8626-B8AB3954B9BF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,10 @@
     <t>Fakultas TIK</t>
   </si>
   <si>
-    <t>Real Nigg</t>
+    <t>Haikal Ghiffari</t>
   </si>
   <si>
-    <t>XIAXIAANY</t>
+    <t>Sandra Agnes</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,7 +390,7 @@
         <v>2</v>
       </c>
       <c r="C1">
-        <v>5111840000033</v>
+        <v>5111840000001</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -403,11 +403,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>511184000077</v>
+        <v>5111840000002</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>

</xml_diff>